<commit_message>
Make identical to version referenced in paper.
See `https://doi.org/10.6084/m9.figshare.17009003.v8`. According to
modification dates, that one is more up-to-date.
</commit_message>
<xml_diff>
--- a/CCTrans_evaluation/Test question corpus.xlsx
+++ b/CCTrans_evaluation/Test question corpus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\CCTrans_evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\soliscom.uu.nl\Users\5621909\My Documents\Desktop\CCTransformationExtraction-main\CCTrans_evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0C8058-1D2A-4D49-99D4-D42D494CBBAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80C0B06-8E59-4B97-AF95-9EE16FA54CB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{E47F8535-B3FB-4347-B625-C78CF20A913A}"/>
   </bookViews>
@@ -612,7 +612,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -652,12 +652,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -717,7 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -743,14 +737,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1076,14 +1067,14 @@
   <dimension ref="A1:C135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A135"/>
+      <selection activeCell="C53" sqref="C53:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="143.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="143.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1390,7 +1381,7 @@
       <c r="B28" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1665,7 +1656,7 @@
       <c r="B53" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C53" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1676,7 +1667,7 @@
       <c r="B54" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1687,7 +1678,7 @@
       <c r="B55" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1731,7 +1722,7 @@
       <c r="B59" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2347,7 +2338,7 @@
       <c r="B115" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C115" s="11" t="s">
+      <c r="C115" s="10" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2457,7 +2448,7 @@
       <c r="B125" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C125" s="12" t="s">
+      <c r="C125" s="11" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>